<commit_message>
test case 5 and 6
</commit_message>
<xml_diff>
--- a/outputs-50-families-6-games.xlsx
+++ b/outputs-50-families-6-games.xlsx
@@ -6831,22 +6831,22 @@
         <v>13</v>
       </c>
       <c r="AI3" t="n">
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="AJ3" t="n">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="AK3" t="n">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="AL3" t="n">
-        <v>1</v>
+        <v>58</v>
       </c>
       <c r="AM3" t="n">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="AN3" t="n">
-        <v>2</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4">
@@ -6946,22 +6946,22 @@
         <v>33</v>
       </c>
       <c r="AI4" t="n">
-        <v>0</v>
+        <v>143</v>
       </c>
       <c r="AJ4" t="n">
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="AK4" t="n">
-        <v>0</v>
+        <v>172</v>
       </c>
       <c r="AL4" t="n">
-        <v>1</v>
+        <v>189</v>
       </c>
       <c r="AM4" t="n">
-        <v>2</v>
+        <v>145</v>
       </c>
       <c r="AN4" t="n">
-        <v>2</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6">
@@ -7061,19 +7061,19 @@
         <v>0</v>
       </c>
       <c r="AI6" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AJ6" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AK6" t="n">
         <v>0</v>
       </c>
       <c r="AL6" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AM6" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="AN6" t="n">
         <v>2</v>
@@ -7176,22 +7176,22 @@
         <v>6</v>
       </c>
       <c r="AI7" t="n">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="AJ7" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AK7" t="n">
         <v>0</v>
       </c>
       <c r="AL7" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AM7" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="AN7" t="n">
-        <v>0</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8">
@@ -7291,22 +7291,22 @@
         <v>7</v>
       </c>
       <c r="AI8" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="AJ8" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="AK8" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AL8" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="AM8" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="AN8" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9">
@@ -7406,19 +7406,19 @@
         <v>0</v>
       </c>
       <c r="AI9" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AJ9" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AK9" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="AL9" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="AM9" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AN9" t="n">
         <v>0</v>
@@ -7521,19 +7521,19 @@
         <v>0</v>
       </c>
       <c r="AI10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ10" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AK10" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AL10" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AM10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN10" t="n">
         <v>0</v>
@@ -7598,7 +7598,7 @@
         <v>13</v>
       </c>
       <c r="J14" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15">
@@ -7623,7 +7623,7 @@
         <v>33</v>
       </c>
       <c r="J15" t="n">
-        <v>1</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16">
@@ -7648,7 +7648,7 @@
         <v>2</v>
       </c>
       <c r="J16" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17">
@@ -7673,7 +7673,7 @@
         <v>5</v>
       </c>
       <c r="J17" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18">
@@ -7698,7 +7698,7 @@
         <v>4</v>
       </c>
       <c r="J18" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19">
@@ -7723,7 +7723,7 @@
         <v>2</v>
       </c>
       <c r="J19" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20">
@@ -7748,7 +7748,7 @@
         <v>1</v>
       </c>
       <c r="J20" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22">
@@ -7780,7 +7780,7 @@
         <v>23</v>
       </c>
       <c r="J23" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24">
@@ -7805,7 +7805,7 @@
         <v>27</v>
       </c>
       <c r="J24" t="n">
-        <v>2</v>
+        <v>143</v>
       </c>
     </row>
     <row r="25">
@@ -7937,7 +7937,7 @@
         <v>60</v>
       </c>
       <c r="J32" t="n">
-        <v>1</v>
+        <v>84</v>
       </c>
     </row>
     <row r="33">
@@ -7962,7 +7962,7 @@
         <v>70</v>
       </c>
       <c r="J33" t="n">
-        <v>2</v>
+        <v>436</v>
       </c>
     </row>
     <row r="34">
@@ -8423,7 +8423,7 @@
         <v>36</v>
       </c>
       <c r="J19" t="n">
-        <v>3</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20">
@@ -8448,7 +8448,7 @@
         <v>19</v>
       </c>
       <c r="J20" t="n">
-        <v>0</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21">
@@ -8473,7 +8473,7 @@
         <v>14</v>
       </c>
       <c r="J21" t="n">
-        <v>0</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22">
@@ -8498,7 +8498,7 @@
         <v>8</v>
       </c>
       <c r="J22" t="n">
-        <v>2</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23">
@@ -8523,7 +8523,7 @@
         <v>0</v>
       </c>
       <c r="J23" t="n">
-        <v>0</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24">
@@ -8548,7 +8548,7 @@
         <v>0</v>
       </c>
       <c r="J24" t="n">
-        <v>0</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27">
@@ -8580,7 +8580,7 @@
         <v>100</v>
       </c>
       <c r="J28" t="n">
-        <v>3</v>
+        <v>184</v>
       </c>
     </row>
     <row r="29">
@@ -8605,7 +8605,7 @@
         <v>47</v>
       </c>
       <c r="J29" t="n">
-        <v>0</v>
+        <v>191</v>
       </c>
     </row>
     <row r="30">
@@ -8630,7 +8630,7 @@
         <v>34</v>
       </c>
       <c r="J30" t="n">
-        <v>0</v>
+        <v>128</v>
       </c>
     </row>
     <row r="31">
@@ -8655,7 +8655,7 @@
         <v>19</v>
       </c>
       <c r="J31" t="n">
-        <v>2</v>
+        <v>150</v>
       </c>
     </row>
     <row r="32">
@@ -8680,7 +8680,7 @@
         <v>0</v>
       </c>
       <c r="J32" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33">
@@ -8705,7 +8705,7 @@
         <v>0</v>
       </c>
       <c r="J33" t="n">
-        <v>0</v>
+        <v>203</v>
       </c>
     </row>
     <row r="36">
@@ -8741,7 +8741,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AP43"/>
+  <dimension ref="A1:AQ43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:E43"/>
@@ -8882,10 +8882,10 @@
         <v>0</v>
       </c>
       <c r="N7" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="O7" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="P7" t="n">
         <v>0</v>
@@ -8894,70 +8894,70 @@
         <v>0</v>
       </c>
       <c r="R7" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="S7" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="T7" t="n">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="U7" t="n">
         <v>0</v>
       </c>
       <c r="V7" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="W7" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="X7" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="Y7" t="n">
         <v>0</v>
       </c>
       <c r="Z7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA7" t="n">
         <v>0</v>
       </c>
       <c r="AB7" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AC7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD7" t="n">
         <v>0</v>
       </c>
       <c r="AE7" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AF7" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AG7" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AH7" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="AI7" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="AJ7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK7" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AL7" t="n">
         <v>0</v>
       </c>
       <c r="AM7" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AN7" t="n">
         <v>0</v>
@@ -8966,7 +8966,10 @@
         <v>0</v>
       </c>
       <c r="AP7" t="n">
-        <v>28</v>
+        <v>0</v>
+      </c>
+      <c r="AQ7" t="n">
+        <v>-135</v>
       </c>
     </row>
     <row r="8">
@@ -10502,7 +10505,7 @@
     </row>
     <row r="7">
       <c r="B7" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>